<commit_message>
Added ability to update docs & background upload of sales
</commit_message>
<xml_diff>
--- a/Export Docs_Small.xlsx
+++ b/Export Docs_Small.xlsx
@@ -9,11 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9630" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9630"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="57">
   <si>
     <t>BAMPORINEZA EMMANUEL</t>
   </si>
@@ -196,48 +195,6 @@
   </si>
   <si>
     <t xml:space="preserve">AGENT </t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Transaction date</t>
-  </si>
-  <si>
-    <t>Format</t>
-  </si>
-  <si>
-    <t>DD-MM-YYYY</t>
-  </si>
-  <si>
-    <t>Customer name</t>
-  </si>
-  <si>
-    <t>Max 50 characters</t>
-  </si>
-  <si>
-    <t>The delivery note ref</t>
-  </si>
-  <si>
-    <t>Max 20 characters</t>
-  </si>
-  <si>
-    <t>Vehicler registration number</t>
-  </si>
-  <si>
-    <t>Agent code</t>
-  </si>
-  <si>
-    <t>Destination country name/code</t>
-  </si>
-  <si>
-    <t>Total value</t>
-  </si>
-  <si>
-    <t>QTY9TONS</t>
-  </si>
-  <si>
-    <t>Quantity in tons</t>
   </si>
 </sst>
 </file>
@@ -616,8 +573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -993,144 +950,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D12"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.25" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B2" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B3" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B4" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5" t="s">
-        <v>65</v>
-      </c>
-      <c r="D5" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B6" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B7" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B8" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B9" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C9" t="s">
-        <v>70</v>
-      </c>
-      <c r="D9" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B10" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C10" t="s">
-        <v>68</v>
-      </c>
-      <c r="D10" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B11" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C11" t="s">
-        <v>67</v>
-      </c>
-      <c r="D11" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B12" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C12" t="s">
-        <v>66</v>
-      </c>
-      <c r="D12" t="s">
-        <v>64</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Added trailer vehicle #
</commit_message>
<xml_diff>
--- a/Export Docs_Small.xlsx
+++ b/Export Docs_Small.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="59">
   <si>
     <t>BAMPORINEZA EMMANUEL</t>
   </si>
@@ -194,7 +194,13 @@
     <t>DESTINATION</t>
   </si>
   <si>
-    <t xml:space="preserve">AGENT </t>
+    <t>VEH# TRAILER</t>
+  </si>
+  <si>
+    <t>TR20282</t>
+  </si>
+  <si>
+    <t>TR272625</t>
   </si>
 </sst>
 </file>
@@ -574,7 +580,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.375" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -747,7 +753,9 @@
       <c r="J5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="K5" s="3"/>
+      <c r="K5" s="3" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
@@ -879,7 +887,9 @@
       <c r="J9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="K9" s="3"/>
+      <c r="K9" s="3" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="4">

</xml_diff>